<commit_message>
Modified R&O Template to remove deduction of opportunities from risks
</commit_message>
<xml_diff>
--- a/script-risk-register/R&O Report Template.xlsx
+++ b/script-risk-register/R&O Report Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8536B5A2-8E23-F843-90BC-5D9765C1E246}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7ED326-4BFC-BC47-BAD0-BD060E064E15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="500" windowWidth="32440" windowHeight="20400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="500" windowWidth="32440" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -2616,7 +2616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3:H3"/>
     </sheetView>
   </sheetViews>
@@ -2661,7 +2661,7 @@
       <c r="C3" s="59"/>
       <c r="D3" s="59"/>
       <c r="E3" s="58">
-        <f>'Table 1'!H7-'Table 2'!H7</f>
+        <f>'Table 1'!H7</f>
         <v>0</v>
       </c>
       <c r="F3" s="58"/>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="C14" s="32">
         <f ca="1">TODAY()</f>
-        <v>44208</v>
+        <v>44307</v>
       </c>
       <c r="D14" s="35"/>
       <c r="E14" s="15" t="s">
@@ -4196,7 +4196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -4354,7 +4354,7 @@
       </c>
       <c r="C14" s="32">
         <f ca="1">TODAY()</f>
-        <v>44208</v>
+        <v>44307</v>
       </c>
       <c r="D14" s="35"/>
       <c r="E14" s="16" t="s">

</xml_diff>

<commit_message>
Wbs Code mapping and changed template to remove references to dollars
</commit_message>
<xml_diff>
--- a/script-risk-register/R&O Report Template.xlsx
+++ b/script-risk-register/R&O Report Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7ED326-4BFC-BC47-BAD0-BD060E064E15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD302835-B156-6748-A55E-B87A614FD3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="500" windowWidth="32440" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="500" windowWidth="32440" windowHeight="20400" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Table 7" sheetId="17" r:id="rId7"/>
     <sheet name="Table 8" sheetId="13" r:id="rId8"/>
     <sheet name="Table 9" sheetId="15" r:id="rId9"/>
-    <sheet name="Fig. 1 Running Graph" sheetId="8" r:id="rId10"/>
+    <sheet name="Fig. 1 Running Graph" sheetId="8" state="hidden" r:id="rId10"/>
     <sheet name="All Active Risks" sheetId="16" r:id="rId11"/>
     <sheet name="All Non-Active Risks" sheetId="19" r:id="rId12"/>
     <sheet name="All Mitigations" sheetId="18" r:id="rId13"/>
@@ -647,7 +647,6 @@
     <xf numFmtId="164" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -662,16 +661,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -714,12 +707,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -739,12 +726,8 @@
     <xf numFmtId="14" fontId="18" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -809,6 +792,23 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="17" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="18" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2616,7 +2616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3:H3"/>
     </sheetView>
   </sheetViews>
@@ -2626,83 +2626,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="str">
+      <c r="A2" s="49" t="str">
         <f>IF('Table 1'!H7=0,"This file is the template that the Python ReportData script will use to format its output.
 Go through each tab to find the relevant information for that section of the report.","This file is the generated report data from the Report Data Python script.
 Copy the relevant tables into the Word document to create the report.")</f>
         <v>This file is the template that the Python ReportData script will use to format its output.
 Go through each tab to find the relevant information for that section of the report.</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="58">
+      <c r="A3" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="51">
         <f>'Table 1'!H7</f>
         <v>0</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="60"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="60"/>
-      <c r="B6" s="62" t="s">
+      <c r="A6" s="53"/>
+      <c r="B6" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2760,554 +2760,554 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>41775</v>
       </c>
-      <c r="B2" s="53">
-        <v>0</v>
-      </c>
-      <c r="C2" s="53">
-        <v>0</v>
-      </c>
-      <c r="D2" s="53">
-        <v>0</v>
-      </c>
-      <c r="E2" s="53">
-        <v>0</v>
-      </c>
-      <c r="F2" s="53">
-        <v>0</v>
-      </c>
-      <c r="G2" s="53">
+      <c r="B2" s="46">
+        <v>0</v>
+      </c>
+      <c r="C2" s="46">
+        <v>0</v>
+      </c>
+      <c r="D2" s="46">
+        <v>0</v>
+      </c>
+      <c r="E2" s="46">
+        <v>0</v>
+      </c>
+      <c r="F2" s="46">
+        <v>0</v>
+      </c>
+      <c r="G2" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="N38" s="3"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="N39" s="3"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="N39" s="2"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="N40" s="3"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="N40" s="2"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="N41" s="3"/>
+      <c r="A41" s="3"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="N41" s="2"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="N42" s="3"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="N42" s="2"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="A43" s="3"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="A44" s="3"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="A45" s="3"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="A46" s="3"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
+      <c r="A50" s="3"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="4"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="4"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
+      <c r="A52" s="3"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
+      <c r="A53" s="3"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="A54" s="3"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="47"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
+      <c r="A55" s="40"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="47"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
+      <c r="A56" s="40"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="47"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
+      <c r="A57" s="40"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="47"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="47"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
+      <c r="A59" s="40"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="47"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
+      <c r="A60" s="40"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3322,7 +3322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -3379,337 +3379,337 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="44"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="89" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="16">
         <f>_xlfn.IFNA(INDEX($M$11:$P$17,MATCH($A3,$L$11:$L$17,0),MATCH(B$2,$M$11:$P$11,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="16">
         <f t="shared" ref="C3:E6" si="0">_xlfn.IFNA(INDEX($M$11:$P$17,MATCH($A3,$L$11:$L$17,0),MATCH(C$2,$M$11:$P$11,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F3" s="50">
+      <c r="F3" s="43">
         <f t="shared" ref="F3:I6" si="1">_xlfn.IFNA(INDEX(M$3:M$6,MATCH($A3,$L$3:$L$6,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="50">
+      <c r="G3" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H3" s="50">
+      <c r="H3" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I3" s="50">
+      <c r="I3" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="16">
         <f t="shared" ref="B4:B6" si="2">_xlfn.IFNA(INDEX($M$11:$P$17,MATCH($A4,$L$11:$L$17,0),MATCH(B$2,$M$11:$P$11,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F4" s="50">
+      <c r="F4" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H4" s="50">
+      <c r="H4" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I4" s="50">
+      <c r="I4" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L4" s="26" t="s">
+      <c r="L4" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F5" s="50">
+      <c r="F5" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G5" s="50">
+      <c r="G5" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H5" s="50">
+      <c r="H5" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I5" s="50">
+      <c r="I5" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L5" s="26" t="s">
+      <c r="L5" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="50">
+      <c r="F6" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G6" s="50">
+      <c r="G6" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H6" s="50">
+      <c r="H6" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I6" s="50">
+      <c r="I6" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
     </row>
     <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="17">
         <f t="shared" ref="B7:I7" si="3">SUM(B3:B6)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F7" s="51">
+      <c r="F7" s="44">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G7" s="51">
+      <c r="G7" s="44">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H7" s="51">
+      <c r="H7" s="44">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I7" s="51">
+      <c r="I7" s="44">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L7" s="26" t="s">
+      <c r="L7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="54">
+      <c r="M7" s="47">
         <f>SUM(M3:M6)</f>
         <v>0</v>
       </c>
-      <c r="N7" s="54">
+      <c r="N7" s="47">
         <f>SUM(N3:N6)</f>
         <v>0</v>
       </c>
-      <c r="O7" s="54">
+      <c r="O7" s="47">
         <f>SUM(O3:O6)</f>
         <v>0</v>
       </c>
-      <c r="P7" s="54">
+      <c r="P7" s="47">
         <f>SUM(P3:P6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L11" s="43" t="s">
+      <c r="L11" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="43"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L15" s="43"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="43"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L16" s="43"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="43"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3740,250 +3740,250 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
     </row>
     <row r="2" spans="1:15" ht="89" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="16">
         <f t="shared" ref="B3:E6" si="0">_xlfn.IFNA(INDEX($L$12:$O$16,MATCH($A3,$K$12:$K$16,0),MATCH(B$2,$L$11:$O$11,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="48">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="41">
         <f>_xlfn.IFNA(INDEX($L$3:$L$6,MATCH(A3,$K$3:$K$6,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="28"/>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="48">
+      <c r="H4" s="41">
         <f>_xlfn.IFNA(INDEX($L$3:$L$6,MATCH(A4,$K$3:$K$6,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="28"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="48">
+      <c r="H5" s="41">
         <f>_xlfn.IFNA(INDEX($L$3:$L$6,MATCH(A5,$K$3:$K$6,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="28"/>
+      <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="48">
+      <c r="H6" s="41">
         <f>_xlfn.IFNA(INDEX($L$3:$L$6,MATCH(A6,$K$3:$K$6,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="28"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="17">
         <f>SUM(B3:B6)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="17">
         <f>SUM(C3:C6)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="17">
         <f>SUM(D3:D6)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="17">
         <f>SUM(E3:E6)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="49">
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="42">
         <f>SUM(H3:H6)</f>
         <v>0</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="55">
+      <c r="L7" s="48">
         <f>SUM(L3:L6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K11" s="43" t="s">
+      <c r="K11" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="43"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K16" s="43"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="43"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3998,7 +3998,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:G14"/>
+      <selection activeCell="G4" sqref="G4:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4013,173 +4013,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="7"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>7</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="12">
+      <c r="A11" s="10">
         <v>8</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
+      <c r="A12" s="10">
         <v>9</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="12">
+      <c r="A13" s="10">
         <v>10</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
     </row>
     <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
-      <c r="B14" s="31" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="27">
         <f ca="1">TODAY()</f>
-        <v>44307</v>
-      </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="15" t="s">
+        <v>44369</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="45">
         <f>SUM(F4:F13)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="52">
+      <c r="G14" s="45">
         <f>SUM(G4:G13)</f>
         <v>0</v>
       </c>
@@ -4197,7 +4197,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F4" sqref="F4:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4211,156 +4211,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="12">
+      <c r="A4" s="10">
         <v>1</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="29"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="63"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
+      <c r="A5" s="10">
         <v>2</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="29"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="63"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
+      <c r="A6" s="10">
         <v>3</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="29"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="63"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
+      <c r="A7" s="10">
         <v>4</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="29"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="63"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="12">
+      <c r="A8" s="10">
         <v>5</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="29"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="63"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="12">
+      <c r="A9" s="10">
         <v>6</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="29"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="63"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
+      <c r="A10" s="10">
         <v>7</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="29"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="63"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="12">
+      <c r="A11" s="10">
         <v>8</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="29"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="63"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
+      <c r="A12" s="10">
         <v>9</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="29"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="63"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="12">
+      <c r="A13" s="10">
         <v>10</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="29"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="63"/>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
-      <c r="B14" s="31" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="27">
         <f ca="1">TODAY()</f>
-        <v>44307</v>
-      </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="16" t="s">
+        <v>44369</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="45">
         <f>SUM(F4:F13)</f>
         <v>0</v>
       </c>
@@ -4379,39 +4379,39 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12" style="25" customWidth="1"/>
+    <col min="1" max="1" width="12" style="22" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="64.5" style="8" customWidth="1"/>
-    <col min="5" max="6" width="10.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="64.5" style="8" customWidth="1"/>
+    <col min="4" max="4" width="64.5" style="7" customWidth="1"/>
+    <col min="5" max="6" width="10.33203125" style="65" customWidth="1"/>
+    <col min="7" max="7" width="64.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="21" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4425,49 +4425,49 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="39" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" style="39" customWidth="1"/>
-    <col min="3" max="3" width="28.5" style="39" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="39" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="40" customWidth="1"/>
-    <col min="6" max="6" width="13" style="39" customWidth="1"/>
-    <col min="7" max="10" width="14.33203125" style="41" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="33" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="33" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="33" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="34" customWidth="1"/>
+    <col min="6" max="6" width="13" style="33" customWidth="1"/>
+    <col min="7" max="10" width="14.33203125" style="67" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="66" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4489,26 +4489,26 @@
     <col min="3" max="3" width="77.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="81.33203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="81.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="21" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4589,26 +4589,26 @@
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="56.1640625" style="8" customWidth="1"/>
+    <col min="5" max="6" width="56.1640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="21" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>